<commit_message>
Code Optimized, added error messages
</commit_message>
<xml_diff>
--- a/Extra/Prescaler Stuff.xlsx
+++ b/Extra/Prescaler Stuff.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wede\Documents\GitHub\Plexim_2k18\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wede\Documents\GitHub\Plexim_2k18\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF12382-E0CD-4747-BB87-0FA659561CBC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C164849-BD26-4AFA-A3BA-E9C6A98002A5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{A4FC6783-6641-4D77-88C6-69B9A5920BF9}"/>
   </bookViews>
@@ -19,6 +19,11 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -404,7 +409,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FAE368-E824-4D5E-BF74-03A3063E11A0}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
@@ -414,8 +419,9 @@
   <cols>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -440,95 +446,112 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <f>E2/A2*1000000</f>
-        <v>2000000</v>
+        <f>E3/A2*1000000</f>
+        <v>16000000</v>
       </c>
       <c r="C2" s="1">
-        <f>G2/D2-1</f>
-        <v>399999.00000000006</v>
+        <f>G3/D2-1</f>
+        <v>65599999</v>
       </c>
       <c r="D2">
         <f>1/B2</f>
-        <v>4.9999999999999998E-7</v>
-      </c>
-      <c r="E2">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>0.2</v>
+        <v>6.2499999999999997E-8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <f>E2/A3*1000000</f>
-        <v>1000000</v>
+        <f>E3/A3*1000000</f>
+        <v>2000000</v>
       </c>
       <c r="C3" s="1">
-        <f>G2/D3-1</f>
-        <v>199999.00000000003</v>
+        <f>G3/D3-1</f>
+        <v>8199999</v>
       </c>
       <c r="D3">
         <f>1/B3</f>
-        <v>9.9999999999999995E-7</v>
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <f>E2/A4*1000000</f>
-        <v>250000</v>
+        <f>E3/A4*1000000</f>
+        <v>1000000</v>
       </c>
       <c r="C4" s="1">
-        <f>G2/D4-1</f>
-        <v>49999.000000000007</v>
+        <f>G3/D4-1</f>
+        <v>4099999</v>
       </c>
       <c r="D4">
         <f>1/B4</f>
-        <v>3.9999999999999998E-6</v>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="B5">
-        <f>E2/A5*1000000</f>
-        <v>62500</v>
+        <f>E3/A5*1000000</f>
+        <v>250000</v>
       </c>
       <c r="C5" s="1">
-        <f>G2/D5-1</f>
-        <v>12499.000000000002</v>
+        <f>G3/D5-1</f>
+        <v>1024999</v>
       </c>
       <c r="D5">
         <f>1/B5</f>
-        <v>1.5999999999999999E-5</v>
+        <v>3.9999999999999998E-6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1024</v>
+        <v>256</v>
       </c>
       <c r="B6">
-        <f>E2/A6*1000000</f>
-        <v>15625</v>
+        <f>E3/A6*1000000</f>
+        <v>62500</v>
       </c>
       <c r="C6" s="1">
-        <f>G2/D6-1</f>
-        <v>3124.0000000000005</v>
+        <f>G3/D6-1</f>
+        <v>256249</v>
       </c>
       <c r="D6">
         <f>1/B6</f>
+        <v>1.5999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1024</v>
+      </c>
+      <c r="B7">
+        <f>E3/A7*1000000</f>
+        <v>15625</v>
+      </c>
+      <c r="C7" s="1">
+        <f>G3/D7-1</f>
+        <v>64061.5</v>
+      </c>
+      <c r="D7">
+        <f>1/B7</f>
         <v>6.3999999999999997E-5</v>
       </c>
     </row>

</xml_diff>